<commit_message>
fijado bug, asignaba horas a tareas del día sin comprobar si había llegado al límite
</commit_message>
<xml_diff>
--- a/2021-04-12_1210_carga_horas_2020_FEVEL_relleno.xlsx
+++ b/2021-04-12_1210_carga_horas_2020_FEVEL_relleno.xlsx
@@ -2189,10 +2189,10 @@
         <v>0.5</v>
       </c>
       <c r="D37" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E37" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F37" s="6" t="n">
         <v>0</v>
@@ -2452,10 +2452,10 @@
         <v>1</v>
       </c>
       <c r="C44" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D44" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E44" s="6" t="n">
         <v>0</v>
@@ -2487,10 +2487,10 @@
         </is>
       </c>
       <c r="B45" s="6" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C45" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D45" s="6" t="n">
         <v>0</v>
@@ -2534,7 +2534,7 @@
         <v>0.5</v>
       </c>
       <c r="E46" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F46" s="6" t="n">
         <v>0</v>
@@ -2566,13 +2566,13 @@
         <v>0.5</v>
       </c>
       <c r="C47" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D47" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E47" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F47" s="6" t="n">
         <v>0</v>
@@ -2604,7 +2604,7 @@
         <v>1</v>
       </c>
       <c r="C48" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D48" s="6" t="n">
         <v>0</v>
@@ -2832,13 +2832,13 @@
         <v>0.5</v>
       </c>
       <c r="C54" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D54" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E54" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F54" s="6" t="n">
         <v>0</v>
@@ -3022,10 +3022,10 @@
         <v>1</v>
       </c>
       <c r="C59" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D59" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E59" s="6" t="n">
         <v>0</v>
@@ -3364,13 +3364,13 @@
         <v>0.5</v>
       </c>
       <c r="C68" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D68" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E68" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F68" s="6" t="n">
         <v>0</v>
@@ -3592,7 +3592,7 @@
         <v>1</v>
       </c>
       <c r="C74" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D74" s="6" t="n">
         <v>0</v>
@@ -3630,13 +3630,13 @@
         <v>0.5</v>
       </c>
       <c r="C75" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D75" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E75" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F75" s="6" t="n">
         <v>0</v>
@@ -3671,10 +3671,10 @@
         <v>0.5</v>
       </c>
       <c r="D76" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E76" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F76" s="6" t="n">
         <v>0</v>
@@ -3785,10 +3785,10 @@
         <v>0.5</v>
       </c>
       <c r="D79" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E79" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F79" s="6" t="n">
         <v>0</v>
@@ -3896,16 +3896,16 @@
         <v>0.5</v>
       </c>
       <c r="C82" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D82" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E82" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F82" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G82" s="6" t="n">
         <v>0</v>
@@ -4051,10 +4051,10 @@
         <v>0.5</v>
       </c>
       <c r="D86" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E86" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F86" s="6" t="n">
         <v>0</v>
@@ -4317,10 +4317,10 @@
         <v>0.5</v>
       </c>
       <c r="D93" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E93" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F93" s="6" t="n">
         <v>0</v>
@@ -4583,10 +4583,10 @@
         <v>0.5</v>
       </c>
       <c r="D100" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E100" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F100" s="6" t="n">
         <v>0</v>
@@ -4618,10 +4618,10 @@
         <v>1</v>
       </c>
       <c r="C101" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D101" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E101" s="6" t="n">
         <v>0</v>
@@ -5150,7 +5150,7 @@
         <v>1</v>
       </c>
       <c r="C115" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D115" s="6" t="n">
         <v>0</v>
@@ -5416,10 +5416,10 @@
         <v>1</v>
       </c>
       <c r="C122" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D122" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E122" s="6" t="n">
         <v>0</v>
@@ -5460,7 +5460,7 @@
         <v>0.5</v>
       </c>
       <c r="E123" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F123" s="6" t="n">
         <v>0</v>
@@ -6556,13 +6556,13 @@
         <v>0.5</v>
       </c>
       <c r="C152" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D152" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E152" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F152" s="6" t="n">
         <v>0</v>
@@ -6857,7 +6857,7 @@
         </is>
       </c>
       <c r="B160" s="6" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C160" s="6" t="n">
         <v>0.5</v>
@@ -6869,7 +6869,7 @@
         <v>0.5</v>
       </c>
       <c r="F160" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G160" s="6" t="n">
         <v>0</v>
@@ -7012,7 +7012,7 @@
         <v>1</v>
       </c>
       <c r="C164" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D164" s="6" t="n">
         <v>0</v>
@@ -7886,16 +7886,16 @@
         <v>0.5</v>
       </c>
       <c r="C187" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D187" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E187" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F187" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G187" s="6" t="n">
         <v>0</v>
@@ -8345,10 +8345,10 @@
         <v>0.5</v>
       </c>
       <c r="D199" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E199" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F199" s="6" t="n">
         <v>0</v>
@@ -8418,16 +8418,16 @@
         <v>0.5</v>
       </c>
       <c r="C201" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D201" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E201" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F201" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G201" s="6" t="n">
         <v>0</v>
@@ -8684,10 +8684,10 @@
         <v>0.5</v>
       </c>
       <c r="C208" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D208" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E208" s="6" t="n">
         <v>0</v>
@@ -8725,10 +8725,10 @@
         <v>0.5</v>
       </c>
       <c r="D209" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E209" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F209" s="6" t="n">
         <v>0</v>
@@ -10251,7 +10251,7 @@
         <v>0.5</v>
       </c>
       <c r="F249" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G249" s="6" t="n">
         <v>0</v>
@@ -10280,7 +10280,7 @@
         <v>0.5</v>
       </c>
       <c r="C250" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D250" s="6" t="n">
         <v>0</v>
@@ -10745,7 +10745,7 @@
         <v>0.5</v>
       </c>
       <c r="F262" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G262" s="6" t="n">
         <v>0</v>
@@ -10774,7 +10774,7 @@
         <v>1</v>
       </c>
       <c r="C263" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D263" s="6" t="n">
         <v>0</v>
@@ -10964,10 +10964,10 @@
         <v>1</v>
       </c>
       <c r="C268" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D268" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E268" s="6" t="n">
         <v>0</v>
@@ -11078,13 +11078,13 @@
         <v>0.5</v>
       </c>
       <c r="C271" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D271" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E271" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F271" s="6" t="n">
         <v>0</v>
@@ -11227,7 +11227,7 @@
         </is>
       </c>
       <c r="B275" s="6" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C275" s="6" t="n">
         <v>0.5</v>
@@ -11239,7 +11239,7 @@
         <v>0.5</v>
       </c>
       <c r="F275" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G275" s="6" t="n">
         <v>0</v>
@@ -11277,7 +11277,7 @@
         <v>0.5</v>
       </c>
       <c r="F276" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G276" s="6" t="n">
         <v>0</v>
@@ -11344,16 +11344,16 @@
         <v>0.5</v>
       </c>
       <c r="C278" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D278" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E278" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F278" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G278" s="6" t="n">
         <v>0</v>
@@ -11379,10 +11379,10 @@
         </is>
       </c>
       <c r="B279" s="6" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C279" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D279" s="6" t="n">
         <v>0</v>
@@ -11502,7 +11502,7 @@
         <v>0.5</v>
       </c>
       <c r="E282" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F282" s="6" t="n">
         <v>0</v>
@@ -11876,13 +11876,13 @@
         <v>0.5</v>
       </c>
       <c r="C292" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D292" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E292" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F292" s="6" t="n">
         <v>0</v>
@@ -11914,7 +11914,7 @@
         <v>1</v>
       </c>
       <c r="C293" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D293" s="6" t="n">
         <v>0</v>
@@ -12373,10 +12373,10 @@
         <v>0.5</v>
       </c>
       <c r="D305" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E305" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F305" s="6" t="n">
         <v>0</v>
@@ -12408,13 +12408,13 @@
         <v>0.5</v>
       </c>
       <c r="C306" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D306" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E306" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F306" s="6" t="n">
         <v>0</v>
@@ -12636,7 +12636,7 @@
         <v>1</v>
       </c>
       <c r="C312" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D312" s="6" t="n">
         <v>0</v>
@@ -12674,16 +12674,16 @@
         <v>0.5</v>
       </c>
       <c r="C313" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D313" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E313" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F313" s="6" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G313" s="6" t="n">
         <v>0</v>
@@ -12718,7 +12718,7 @@
         <v>0.5</v>
       </c>
       <c r="E314" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F314" s="6" t="n">
         <v>0</v>
@@ -13396,7 +13396,7 @@
         <v>1</v>
       </c>
       <c r="C332" s="6" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D332" s="6" t="n">
         <v>0</v>

</xml_diff>